<commit_message>
New test cases added - Still in progress
</commit_message>
<xml_diff>
--- a/App_QC_Regression_Test_Case.xlsx
+++ b/App_QC_Regression_Test_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\BluePrint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268EF4D6-7F7B-4810-BC33-BADD69719504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70F61A6-F60E-4CB3-9C6A-06774ED89EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="20730" windowHeight="11160" tabRatio="892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="20730" windowHeight="11160" tabRatio="892" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Page" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="653">
   <si>
     <t>Test Area</t>
   </si>
@@ -2271,6 +2271,231 @@
   <si>
     <t xml:space="preserve">1) Appropriate certinty score, file list, error list cluster list etc should be visible
 2) Preparation Status should be properly displayed and user should be able to download the csv file without error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting pdf with table and then Select Table Data label
+3) Position the selector box on the table and click save
+</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different bounding box step for images in a cluster</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different data labels step for pdf file with tables in a cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting image and then Select Bounding box Data label
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) User should be able to see multiple fields to select x coordinate, y coordinate z cordinate page index etc. In the plan, view user should be able to see selector box.
+3) New Bounding data step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) User should be able to see multiple fields to select x coordinate, y coordinate z cordinate page index etc. In the plan, view user should be able to see selector box.
+3) New table data lebel should be saved for the document.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting docx and then Select ParseTreeQuery
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) User should be able to see multiple fields to select x coordinate, y coordinate z cordinate page index etc. In the plan, view user should be able to see selector box.
+3) New Parse Tree Query step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different Parse tree query step for docx file in a cluster</t>
+  </si>
+  <si>
+    <t>Verify that adding Create Data Atom next step saves the value to one of the data labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Under the bounding box step,  add a CreateDataAtom next step </t>
+  </si>
+  <si>
+    <t>1) It must save the value to one of the data labels</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different Regex Step in a cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting anyfile and then Select Regex
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) TBD
+3) New Regex step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different next step selector Step in a cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting anyfile and then Select Next Step Selector
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) TBD
+3) New NextStepSelector step should be saved for the document.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user create a draft plan, click on Tree view
+2) Click on plan view by selecting anyfile and then Select PassThrough
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to create different PassThrough Step in a cluster</t>
+  </si>
+  <si>
+    <t>1) User should be able to see steps label and add new step dropdown.
+2) TBD
+3) New PassThrough step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>Verify that user can see preview on the plan for few document</t>
+  </si>
+  <si>
+    <t>1) Once all steps are creaded click on Preview checkmark in middle of the page</t>
+  </si>
+  <si>
+    <t>1) user should be able to see preview of the the page</t>
+  </si>
+  <si>
+    <t>Verify that user can find appropriate visibility on Available/Plan/Preview action on the plan</t>
+  </si>
+  <si>
+    <t>1) Once all steps are creaded click on Available/Plan/Preview checkmark in middle of the page</t>
+  </si>
+  <si>
+    <t>1) Appropriate selection should be seen on the selected files. 
+2) Selected file should match with the preview visible.</t>
+  </si>
+  <si>
+    <t>Verifty that user should not be able to see cluster list  in the collection details page</t>
+  </si>
+  <si>
+    <t>1) Now login to blue print application and select the collection whose cluster has been added with the steps as mentioned in above test case</t>
+  </si>
+  <si>
+    <t>1) User being on a Collection detail page, cluster with pending status should no t be visible.
+2) Document download, certainty information and extraction should not be visible for any cluster.
+3) Collection metrics should not be affected in any condition</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to modify different data labels step for pdf file with tables in a cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user select a draft plan, click on Tree view
+2) Click on plan view by selecting pdf with table and then Select Table Data label
+3) Position the selector box on the table and click save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user select a draft plan, click on Tree view
+2) Click on plan view by selecting image and then Select Bounding box Data label
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to modify different bounding box step for images in a cluster</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to modify different Parse tree query step for docx file in a cluster</t>
+  </si>
+  <si>
+    <t>Verify that modifying Create Data Atom next step saves the value to one of the data labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Under the bounding box step,  modify existing  CreateDataAtom next step </t>
+  </si>
+  <si>
+    <t>Verify that user should be able to modify different Regex Step in a cluster</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to modify different PassThrough Step in a cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user select a draft plan, click on Tree view
+2) Click on plan view by selecting anyfile and then Select PassThrough
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In AI tool, once user select a draft plan, click on Tree view
+2) Click on plan view by selecting anyfile and then Select Regex
+3) Position the selector box on the image and click save
+</t>
+  </si>
+  <si>
+    <t>1) User should be able to see existing steps label and add new step dropdown.
+2) User should be able to see multiple fields to select x coordinate, y coordinate z cordinate page index etc. In the plan, view user should be able to see selector box.
+3) Existing Table data lebel should be saved with updated values for the document.</t>
+  </si>
+  <si>
+    <t>1) User should be able to see existingsteps label and add new step dropdown.
+2) User should be able to see multiple fields to select x coordinate, y coordinate z cordinate page index etc. In the plan, view user should be able to see selector box.
+3) Existing Bounding data step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>1) User should be able to see existing steps label and add new step dropdown.
+2) TBD
+3) Existing PassThrough step should be saved for the document.</t>
+  </si>
+  <si>
+    <t>1) Once all steps are Updated click on Available/Plan/Preview checkmark in middle of the page</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to move the files that are in Stage section to Unstaged section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) List of Unstaged files should be visible
+2) User should be able to see popup with Stage button
+3) File should be removed from the Unstaged section and must be moved from Unstage section.to Staged section
+</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to Injest and Activate the cluster for all staqed files</t>
+  </si>
+  <si>
+    <t>1) On the right botton area, look for Injest and Activate button
+2) Click on Injest and activate button</t>
+  </si>
+  <si>
+    <t>1) Injest and activate button should be visible
+2) Injest and Activate should be success. To verify navigate to django admin &gt;&gt;Home&gt;&gt;Injest result, new result should be created, is executed in a background and gets a status value complete.</t>
+  </si>
+  <si>
+    <t>1) On the left bottom area, expand Unstaged folder
+2) Right click on a file
+3) Click on Stage button and then expand staged folder
+Note: This feature is also workable in the folder level. Right click on Unstaged folder and Stage the file should move all the file from Unstaged to staged folder.
+For now keep few files in Unstaged folder.</t>
+  </si>
+  <si>
+    <t>Verifty that list of files that are not Staged are remaining in Unstaged folder</t>
+  </si>
+  <si>
+    <t>1) Check for the files that are not injested and were not staged in the step above</t>
+  </si>
+  <si>
+    <t>1) Files which are not injested or staged should remain in the Unstaged folder</t>
   </si>
 </sst>
 </file>
@@ -2696,7 +2921,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2992,6 +3217,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3028,6 +3259,15 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3037,22 +3277,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3063,19 +3294,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3088,7 +3306,56 @@
     <cellStyle name="Normal 2 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="224">
+  <dxfs count="231">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5006,7 +5273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -5053,11 +5320,11 @@
       <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:55" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="115" t="s">
         <v>266</v>
       </c>
-      <c r="B5" s="114"/>
-      <c r="C5" s="115"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="117"/>
       <c r="D5" s="58"/>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -5070,8 +5337,8 @@
       <c r="A6" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="119"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="121"/>
       <c r="D6" s="50"/>
       <c r="P6" s="35"/>
     </row>
@@ -5079,8 +5346,8 @@
       <c r="A7" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="119"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="121"/>
       <c r="D7" s="51"/>
       <c r="P7" s="35"/>
     </row>
@@ -5088,8 +5355,8 @@
       <c r="A8" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="51"/>
       <c r="P8" s="35"/>
     </row>
@@ -5097,8 +5364,8 @@
       <c r="A9" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="119"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="121"/>
       <c r="D9" s="29"/>
       <c r="P9" s="35"/>
     </row>
@@ -5317,10 +5584,10 @@
       <c r="B14" s="53" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="122" t="s">
         <v>263</v>
       </c>
-      <c r="D14" s="121"/>
+      <c r="D14" s="123"/>
       <c r="E14" s="52" t="s">
         <v>264</v>
       </c>
@@ -5384,10 +5651,10 @@
       <c r="B15" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="D15" s="117"/>
+      <c r="D15" s="119"/>
       <c r="E15" s="56"/>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -5441,8 +5708,8 @@
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="57"/>
       <c r="B16" s="55"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="119"/>
       <c r="E16" s="56"/>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
@@ -5530,7 +5797,7 @@
       <c r="A3" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="85"/>
@@ -5555,7 +5822,7 @@
       <c r="A4" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="65" t="s">
@@ -5641,48 +5908,48 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="167" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4">
-    <cfRule type="cellIs" dxfId="160" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5767,7 +6034,7 @@
       <c r="A3" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="85"/>
@@ -5792,7 +6059,7 @@
       <c r="A4" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="65" t="s">
@@ -5878,71 +6145,71 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H6:H7">
-    <cfRule type="cellIs" dxfId="153" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H4">
-    <cfRule type="cellIs" dxfId="146" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="15" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="16" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="17" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="18" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="20" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="139" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6027,7 +6294,7 @@
       <c r="A3" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="85"/>
@@ -6052,7 +6319,7 @@
       <c r="A4" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="65" t="s">
@@ -6180,25 +6447,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H9">
-    <cfRule type="cellIs" dxfId="132" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6283,7 +6550,7 @@
       <c r="A3" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="98"/>
@@ -6308,7 +6575,7 @@
       <c r="A4" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="98"/>
       <c r="D4" s="98"/>
       <c r="E4" s="65" t="s">
@@ -6354,7 +6621,7 @@
       <c r="A6" s="98" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="98"/>
@@ -6379,7 +6646,7 @@
       <c r="A7" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="98"/>
       <c r="D7" s="98"/>
       <c r="E7" s="65" t="s">
@@ -6425,7 +6692,7 @@
       <c r="A9" s="98" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="98"/>
@@ -6450,7 +6717,7 @@
       <c r="A10" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="122"/>
+      <c r="B10" s="124"/>
       <c r="C10" s="98"/>
       <c r="D10" s="98"/>
       <c r="E10" s="65" t="s">
@@ -6496,7 +6763,7 @@
       <c r="A12" s="98" t="s">
         <v>284</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="98"/>
@@ -6521,7 +6788,7 @@
       <c r="A13" s="98" t="s">
         <v>285</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="98"/>
       <c r="D13" s="98"/>
       <c r="E13" s="65" t="s">
@@ -6567,7 +6834,7 @@
       <c r="A15" s="98" t="s">
         <v>287</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="98"/>
@@ -6592,7 +6859,7 @@
       <c r="A16" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="B16" s="122"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="98"/>
       <c r="D16" s="98"/>
       <c r="E16" s="65" t="s">
@@ -6638,7 +6905,7 @@
       <c r="A18" s="98" t="s">
         <v>290</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="98"/>
@@ -6663,7 +6930,7 @@
       <c r="A19" s="98" t="s">
         <v>291</v>
       </c>
-      <c r="B19" s="122"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="98"/>
       <c r="D19" s="98"/>
       <c r="E19" s="65" t="s">
@@ -6709,7 +6976,7 @@
       <c r="A21" s="98" t="s">
         <v>293</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="98"/>
@@ -6734,7 +7001,7 @@
       <c r="A22" s="98" t="s">
         <v>453</v>
       </c>
-      <c r="B22" s="122"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="98"/>
       <c r="D22" s="98"/>
       <c r="E22" s="65" t="s">
@@ -6780,7 +7047,7 @@
       <c r="A24" s="98" t="s">
         <v>455</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="98"/>
@@ -6805,7 +7072,7 @@
       <c r="A25" s="98" t="s">
         <v>456</v>
       </c>
-      <c r="B25" s="122"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="98"/>
       <c r="D25" s="98"/>
       <c r="E25" s="65" t="s">
@@ -6851,7 +7118,7 @@
       <c r="A27" s="98" t="s">
         <v>458</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="98"/>
@@ -6876,7 +7143,7 @@
       <c r="A28" s="98" t="s">
         <v>558</v>
       </c>
-      <c r="B28" s="122"/>
+      <c r="B28" s="124"/>
       <c r="C28" s="98"/>
       <c r="D28" s="98"/>
       <c r="E28" s="65" t="s">
@@ -6922,7 +7189,7 @@
       <c r="A30" s="98" t="s">
         <v>560</v>
       </c>
-      <c r="B30" s="122" t="s">
+      <c r="B30" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="98"/>
@@ -6947,7 +7214,7 @@
       <c r="A31" s="98" t="s">
         <v>561</v>
       </c>
-      <c r="B31" s="122"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="98"/>
       <c r="D31" s="98"/>
       <c r="E31" s="65" t="s">
@@ -6991,245 +7258,245 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H5">
-    <cfRule type="cellIs" dxfId="125" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="78" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="79" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="80" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="81" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="82" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="83" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="84" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H8">
-    <cfRule type="cellIs" dxfId="118" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="57" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="58" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="59" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="60" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="61" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="62" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="63" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="111" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="50" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="51" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="52" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="53" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="54" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="55" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="56" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H14">
-    <cfRule type="cellIs" dxfId="104" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="43" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="44" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="45" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="46" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="47" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="48" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="49" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H17">
-    <cfRule type="cellIs" dxfId="97" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="36" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="37" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="38" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="39" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="40" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="41" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="42" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H20">
-    <cfRule type="cellIs" dxfId="90" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="29" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="31" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="32" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="33" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="34" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="35" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:H23">
-    <cfRule type="cellIs" dxfId="83" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="22" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="24" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="25" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="28" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:H26">
-    <cfRule type="cellIs" dxfId="76" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="15" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="18" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="20" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H29">
-    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H32">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7314,7 +7581,7 @@
       <c r="A3" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="98"/>
@@ -7339,7 +7606,7 @@
       <c r="A4" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="98"/>
       <c r="D4" s="98"/>
       <c r="E4" s="65" t="s">
@@ -7446,25 +7713,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H8">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7549,7 +7816,7 @@
       <c r="A3" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="98"/>
@@ -7574,7 +7841,7 @@
       <c r="A4" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="98"/>
       <c r="D4" s="98"/>
       <c r="E4" s="65" t="s">
@@ -7618,25 +7885,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H5">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7721,11 +7988,11 @@
       <c r="A3" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="136" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="98"/>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="136" t="s">
         <v>273</v>
       </c>
       <c r="E3" s="65" t="s">
@@ -7746,9 +8013,9 @@
       <c r="A4" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="136"/>
+      <c r="B4" s="138"/>
       <c r="C4" s="98"/>
-      <c r="D4" s="136"/>
+      <c r="D4" s="138"/>
       <c r="E4" s="65" t="s">
         <v>505</v>
       </c>
@@ -7767,9 +8034,9 @@
       <c r="A5" s="98" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="135"/>
+      <c r="B5" s="137"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="135"/>
+      <c r="D5" s="137"/>
       <c r="E5" s="65" t="s">
         <v>507</v>
       </c>
@@ -7917,25 +8184,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H11">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8022,7 +8289,7 @@
       <c r="A3" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="98"/>
@@ -8047,7 +8314,7 @@
       <c r="A4" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="98"/>
       <c r="D4" s="98"/>
       <c r="E4" s="65" t="s">
@@ -8091,25 +8358,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H5">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8194,7 +8461,7 @@
       <c r="A3" s="103" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="103"/>
@@ -8219,7 +8486,7 @@
       <c r="A4" s="103" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="103"/>
       <c r="D4" s="103"/>
       <c r="E4" s="65" t="s">
@@ -8367,25 +8634,25 @@
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H10">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8458,7 +8725,7 @@
       <c r="A3" s="112" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="112"/>
@@ -8483,7 +8750,7 @@
       <c r="A4" s="112" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="112"/>
       <c r="D4" s="112"/>
       <c r="E4" s="65" t="s">
@@ -8667,7 +8934,7 @@
       <c r="A3" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="85"/>
@@ -8692,9 +8959,9 @@
       <c r="A4" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="85"/>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="124" t="s">
         <v>260</v>
       </c>
       <c r="E4" s="65" t="s">
@@ -8717,9 +8984,9 @@
       <c r="A5" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="85"/>
-      <c r="D5" s="122"/>
+      <c r="D5" s="124"/>
       <c r="E5" s="65" t="s">
         <v>298</v>
       </c>
@@ -8739,9 +9006,9 @@
       <c r="A6" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="85"/>
-      <c r="D6" s="122"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="65" t="s">
         <v>300</v>
       </c>
@@ -8760,9 +9027,9 @@
       <c r="A7" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="85"/>
-      <c r="D7" s="122"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="65" t="s">
         <v>302</v>
       </c>
@@ -8781,9 +9048,9 @@
       <c r="A8" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="85"/>
-      <c r="D8" s="122"/>
+      <c r="D8" s="124"/>
       <c r="E8" s="65" t="s">
         <v>308</v>
       </c>
@@ -8825,7 +9092,7 @@
       <c r="A10" s="85" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="124" t="s">
         <v>341</v>
       </c>
       <c r="C10" s="85"/>
@@ -8848,7 +9115,7 @@
       <c r="A11" s="85" t="s">
         <v>283</v>
       </c>
-      <c r="B11" s="122"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="85"/>
       <c r="D11" s="85"/>
       <c r="E11" s="65" t="s">
@@ -8869,7 +9136,7 @@
       <c r="A12" s="85" t="s">
         <v>284</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="124" t="s">
         <v>345</v>
       </c>
       <c r="C12" s="85"/>
@@ -8892,7 +9159,7 @@
       <c r="A13" s="85" t="s">
         <v>285</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
       <c r="E13" s="65" t="s">
@@ -8913,11 +9180,11 @@
       <c r="A14" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="126" t="s">
         <v>428</v>
       </c>
       <c r="C14" s="99"/>
-      <c r="D14" s="122"/>
+      <c r="D14" s="124"/>
       <c r="E14" s="100" t="s">
         <v>424</v>
       </c>
@@ -8936,9 +9203,9 @@
       <c r="A15" s="85" t="s">
         <v>287</v>
       </c>
-      <c r="B15" s="124"/>
+      <c r="B15" s="126"/>
       <c r="C15" s="99"/>
-      <c r="D15" s="122"/>
+      <c r="D15" s="124"/>
       <c r="E15" s="100" t="s">
         <v>425</v>
       </c>
@@ -8957,8 +9224,8 @@
       <c r="A16" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="B16" s="124"/>
-      <c r="C16" s="124"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
       <c r="D16" s="85"/>
       <c r="E16" s="100" t="s">
         <v>429</v>
@@ -8978,8 +9245,8 @@
       <c r="A17" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="124"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
       <c r="D17" s="85"/>
       <c r="E17" s="100" t="s">
         <v>432</v>
@@ -9041,7 +9308,7 @@
       <c r="A20" s="85" t="s">
         <v>292</v>
       </c>
-      <c r="B20" s="124"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
       <c r="E20" s="100" t="s">
@@ -9062,7 +9329,7 @@
       <c r="A21" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="B21" s="124"/>
+      <c r="B21" s="126"/>
       <c r="C21" s="85"/>
       <c r="D21" s="85"/>
       <c r="E21" s="100" t="s">
@@ -9081,9 +9348,9 @@
     </row>
     <row r="22" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="69"/>
-      <c r="B22" s="123"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="69"/>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="70"/>
       <c r="F22" s="71"/>
       <c r="G22" s="71"/>
@@ -9092,9 +9359,9 @@
     </row>
     <row r="23" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="69"/>
-      <c r="B23" s="123"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="69"/>
-      <c r="D23" s="123"/>
+      <c r="D23" s="125"/>
       <c r="E23" s="70"/>
       <c r="F23" s="71"/>
       <c r="G23" s="71"/>
@@ -10958,25 +11225,25 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H180">
-    <cfRule type="cellIs" dxfId="223" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="576" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="577" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="577" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="578" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="578" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="579" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="580" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="580" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="581" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="581" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="582" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11147,7 +11414,7 @@
       <c r="A3" s="84" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="84"/>
@@ -11172,9 +11439,9 @@
       <c r="A4" s="84" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="84"/>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="124" t="s">
         <v>260</v>
       </c>
       <c r="E4" s="65" t="s">
@@ -11195,9 +11462,9 @@
       <c r="A5" s="84" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="84"/>
-      <c r="D5" s="122"/>
+      <c r="D5" s="124"/>
       <c r="E5" s="65" t="s">
         <v>298</v>
       </c>
@@ -11216,9 +11483,9 @@
       <c r="A6" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="84"/>
-      <c r="D6" s="122"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="65" t="s">
         <v>300</v>
       </c>
@@ -11237,9 +11504,9 @@
       <c r="A7" s="84" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="84"/>
-      <c r="D7" s="122"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="65" t="s">
         <v>302</v>
       </c>
@@ -11258,7 +11525,7 @@
       <c r="A8" s="84" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="84"/>
       <c r="D8" s="84"/>
       <c r="E8" s="65" t="s">
@@ -11304,48 +11571,48 @@
     <mergeCell ref="D4:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H8">
-    <cfRule type="cellIs" dxfId="216" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="209" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11619,15 +11886,15 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="134" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="130"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="129"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="125"/>
+      <c r="B3" s="130"/>
       <c r="C3" s="11" t="s">
         <v>93</v>
       </c>
@@ -11637,7 +11904,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="126"/>
+      <c r="B4" s="131"/>
       <c r="C4" s="11" t="s">
         <v>95</v>
       </c>
@@ -11647,7 +11914,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="127"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="11" t="s">
         <v>97</v>
       </c>
@@ -11665,7 +11932,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="11" t="s">
         <v>99</v>
       </c>
@@ -11675,7 +11942,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="126"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="11" t="s">
         <v>101</v>
       </c>
@@ -11686,7 +11953,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="126"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="11" t="s">
         <v>103</v>
       </c>
@@ -11696,7 +11963,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="126"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="11" t="s">
         <v>105</v>
       </c>
@@ -11706,7 +11973,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="126"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="11" t="s">
         <v>106</v>
       </c>
@@ -11716,7 +11983,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="126"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="18" t="s">
         <v>107</v>
       </c>
@@ -11735,7 +12002,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="126"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="19" t="s">
         <v>108</v>
       </c>
@@ -11745,7 +12012,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="126"/>
+      <c r="B15" s="131"/>
       <c r="C15" s="11" t="s">
         <v>110</v>
       </c>
@@ -11755,7 +12022,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="126"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="11" t="s">
         <v>112</v>
       </c>
@@ -11765,7 +12032,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="126"/>
+      <c r="B17" s="131"/>
       <c r="C17" s="11" t="s">
         <v>114</v>
       </c>
@@ -11775,7 +12042,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="126"/>
+      <c r="B18" s="131"/>
       <c r="C18" s="11" t="s">
         <v>116</v>
       </c>
@@ -11785,7 +12052,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="126"/>
+      <c r="B19" s="131"/>
       <c r="C19" s="11" t="s">
         <v>118</v>
       </c>
@@ -11795,7 +12062,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="127"/>
+      <c r="B20" s="132"/>
       <c r="C20" s="11" t="s">
         <v>119</v>
       </c>
@@ -11813,7 +12080,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="125"/>
+      <c r="B22" s="130"/>
       <c r="C22" s="11" t="s">
         <v>120</v>
       </c>
@@ -11823,7 +12090,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
-      <c r="B23" s="126"/>
+      <c r="B23" s="131"/>
       <c r="C23" s="11" t="s">
         <v>122</v>
       </c>
@@ -11833,7 +12100,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="126"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="11" t="s">
         <v>124</v>
       </c>
@@ -11843,7 +12110,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-      <c r="B25" s="126"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="11" t="s">
         <v>126</v>
       </c>
@@ -11853,7 +12120,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="126"/>
+      <c r="B26" s="131"/>
       <c r="C26" s="11" t="s">
         <v>127</v>
       </c>
@@ -11863,7 +12130,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="126"/>
+      <c r="B27" s="131"/>
       <c r="C27" s="11" t="s">
         <v>129</v>
       </c>
@@ -11873,7 +12140,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="126"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="11" t="s">
         <v>131</v>
       </c>
@@ -11883,7 +12150,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
-      <c r="B29" s="126"/>
+      <c r="B29" s="131"/>
       <c r="C29" s="11" t="s">
         <v>132</v>
       </c>
@@ -11893,7 +12160,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
-      <c r="B30" s="126"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="16" t="s">
         <v>133</v>
       </c>
@@ -11903,7 +12170,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-      <c r="B31" s="126"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="16" t="s">
         <v>134</v>
       </c>
@@ -11913,7 +12180,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="126"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="16" t="s">
         <v>135</v>
       </c>
@@ -11923,7 +12190,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="126"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="16" t="s">
         <v>136</v>
       </c>
@@ -11933,7 +12200,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="126"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="16" t="s">
         <v>137</v>
       </c>
@@ -11943,7 +12210,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="126"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="16" t="s">
         <v>138</v>
       </c>
@@ -11953,7 +12220,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="126"/>
+      <c r="B36" s="131"/>
       <c r="C36" s="16" t="s">
         <v>139</v>
       </c>
@@ -11963,7 +12230,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="127"/>
+      <c r="B37" s="132"/>
       <c r="C37" s="16" t="s">
         <v>140</v>
       </c>
@@ -11981,7 +12248,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="125"/>
+      <c r="B39" s="130"/>
       <c r="C39" s="11" t="s">
         <v>141</v>
       </c>
@@ -11991,7 +12258,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="126"/>
+      <c r="B40" s="131"/>
       <c r="C40" s="11" t="s">
         <v>143</v>
       </c>
@@ -12001,7 +12268,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="126"/>
+      <c r="B41" s="131"/>
       <c r="C41" s="11" t="s">
         <v>145</v>
       </c>
@@ -12011,7 +12278,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
-      <c r="B42" s="126"/>
+      <c r="B42" s="131"/>
       <c r="C42" s="11" t="s">
         <v>147</v>
       </c>
@@ -12021,7 +12288,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="B43" s="126"/>
+      <c r="B43" s="131"/>
       <c r="C43" s="11" t="s">
         <v>149</v>
       </c>
@@ -12031,7 +12298,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="126"/>
+      <c r="B44" s="131"/>
       <c r="C44" s="11" t="s">
         <v>151</v>
       </c>
@@ -12041,7 +12308,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="126"/>
+      <c r="B45" s="131"/>
       <c r="C45" s="11" t="s">
         <v>152</v>
       </c>
@@ -12051,7 +12318,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
-      <c r="B46" s="126"/>
+      <c r="B46" s="131"/>
       <c r="C46" s="11" t="s">
         <v>153</v>
       </c>
@@ -12061,7 +12328,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
-      <c r="B47" s="126"/>
+      <c r="B47" s="131"/>
       <c r="C47" s="11" t="s">
         <v>154</v>
       </c>
@@ -12071,7 +12338,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="126"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="11" t="s">
         <v>155</v>
       </c>
@@ -12081,7 +12348,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="126"/>
+      <c r="B49" s="131"/>
       <c r="C49" s="11" t="s">
         <v>156</v>
       </c>
@@ -12091,7 +12358,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="126"/>
+      <c r="B50" s="131"/>
       <c r="C50" s="11" t="s">
         <v>157</v>
       </c>
@@ -12101,7 +12368,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
-      <c r="B51" s="126"/>
+      <c r="B51" s="131"/>
       <c r="C51" s="18" t="s">
         <v>158</v>
       </c>
@@ -12119,7 +12386,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="126"/>
+      <c r="B53" s="131"/>
       <c r="C53" s="19" t="s">
         <v>159</v>
       </c>
@@ -12129,7 +12396,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="126"/>
+      <c r="B54" s="131"/>
       <c r="C54" s="11" t="s">
         <v>161</v>
       </c>
@@ -12139,7 +12406,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
-      <c r="B55" s="126"/>
+      <c r="B55" s="131"/>
       <c r="C55" s="11" t="s">
         <v>162</v>
       </c>
@@ -12149,7 +12416,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
-      <c r="B56" s="127"/>
+      <c r="B56" s="132"/>
       <c r="C56" s="11" t="s">
         <v>163</v>
       </c>
@@ -12159,15 +12426,15 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
-      <c r="B57" s="128" t="s">
+      <c r="B57" s="134" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="129"/>
-      <c r="D57" s="130"/>
+      <c r="C57" s="135"/>
+      <c r="D57" s="129"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
-      <c r="B58" s="125"/>
+      <c r="B58" s="130"/>
       <c r="C58" s="11" t="s">
         <v>164</v>
       </c>
@@ -12177,7 +12444,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
-      <c r="B59" s="126"/>
+      <c r="B59" s="131"/>
       <c r="C59" s="11" t="s">
         <v>166</v>
       </c>
@@ -12187,7 +12454,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
-      <c r="B60" s="127"/>
+      <c r="B60" s="132"/>
       <c r="C60" s="11" t="s">
         <v>168</v>
       </c>
@@ -12204,7 +12471,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="125"/>
+      <c r="B62" s="130"/>
       <c r="C62" s="11" t="s">
         <v>170</v>
       </c>
@@ -12214,7 +12481,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
-      <c r="B63" s="126"/>
+      <c r="B63" s="131"/>
       <c r="C63" s="11" t="s">
         <v>171</v>
       </c>
@@ -12224,7 +12491,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
-      <c r="B64" s="126"/>
+      <c r="B64" s="131"/>
       <c r="C64" s="11" t="s">
         <v>172</v>
       </c>
@@ -12234,7 +12501,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
-      <c r="B65" s="127"/>
+      <c r="B65" s="132"/>
       <c r="C65" s="11" t="s">
         <v>173</v>
       </c>
@@ -12244,15 +12511,15 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
-      <c r="B66" s="128" t="s">
+      <c r="B66" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="129"/>
-      <c r="D66" s="130"/>
+      <c r="C66" s="135"/>
+      <c r="D66" s="129"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
-      <c r="B67" s="125"/>
+      <c r="B67" s="130"/>
       <c r="C67" s="11" t="s">
         <v>174</v>
       </c>
@@ -12262,7 +12529,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
-      <c r="B68" s="127"/>
+      <c r="B68" s="132"/>
       <c r="C68" s="11" t="s">
         <v>175</v>
       </c>
@@ -12272,15 +12539,15 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
-      <c r="B69" s="128" t="s">
+      <c r="B69" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="C69" s="129"/>
-      <c r="D69" s="130"/>
+      <c r="C69" s="135"/>
+      <c r="D69" s="129"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
-      <c r="B70" s="125"/>
+      <c r="B70" s="130"/>
       <c r="C70" s="11" t="s">
         <v>176</v>
       </c>
@@ -12290,7 +12557,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
-      <c r="B71" s="126"/>
+      <c r="B71" s="131"/>
       <c r="C71" s="11" t="s">
         <v>177</v>
       </c>
@@ -12300,7 +12567,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
-      <c r="B72" s="126"/>
+      <c r="B72" s="131"/>
       <c r="C72" s="11" t="s">
         <v>178</v>
       </c>
@@ -12310,7 +12577,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
-      <c r="B73" s="127"/>
+      <c r="B73" s="132"/>
       <c r="C73" s="11" t="s">
         <v>179</v>
       </c>
@@ -12320,11 +12587,11 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
-      <c r="B74" s="128" t="s">
+      <c r="B74" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="C74" s="129"/>
-      <c r="D74" s="130"/>
+      <c r="C74" s="135"/>
+      <c r="D74" s="129"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
@@ -12568,15 +12835,15 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
-      <c r="B99" s="128" t="s">
+      <c r="B99" s="134" t="s">
         <v>82</v>
       </c>
-      <c r="C99" s="129"/>
-      <c r="D99" s="130"/>
+      <c r="C99" s="135"/>
+      <c r="D99" s="129"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
-      <c r="B100" s="125"/>
+      <c r="B100" s="130"/>
       <c r="C100" s="11" t="s">
         <v>205</v>
       </c>
@@ -12586,7 +12853,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
-      <c r="B101" s="126"/>
+      <c r="B101" s="131"/>
       <c r="C101" s="11" t="s">
         <v>207</v>
       </c>
@@ -12596,7 +12863,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
-      <c r="B102" s="126"/>
+      <c r="B102" s="131"/>
       <c r="C102" s="11" t="s">
         <v>209</v>
       </c>
@@ -12606,7 +12873,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
-      <c r="B103" s="127"/>
+      <c r="B103" s="132"/>
       <c r="C103" s="11" t="s">
         <v>211</v>
       </c>
@@ -12616,11 +12883,11 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="15"/>
-      <c r="B104" s="131" t="s">
+      <c r="B104" s="127" t="s">
         <v>251</v>
       </c>
-      <c r="C104" s="132"/>
-      <c r="D104" s="130"/>
+      <c r="C104" s="128"/>
+      <c r="D104" s="129"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
@@ -12634,6 +12901,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B67:B68"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B62:B65"/>
     <mergeCell ref="B3:B5"/>
@@ -12650,13 +12924,6 @@
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B39:B51"/>
     <mergeCell ref="B22:B37"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B67:B68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12730,7 +12997,7 @@
       <c r="A3" s="84" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="84"/>
@@ -12755,7 +13022,7 @@
       <c r="A4" s="84" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="84"/>
       <c r="D4" s="84"/>
       <c r="E4" s="65" t="s">
@@ -12903,25 +13170,25 @@
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H10">
-    <cfRule type="cellIs" dxfId="202" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13007,7 +13274,7 @@
       <c r="A3" s="84" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="84"/>
@@ -13032,7 +13299,7 @@
       <c r="A4" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="84"/>
       <c r="D4" s="84"/>
       <c r="E4" s="65" t="s">
@@ -13053,7 +13320,7 @@
       <c r="A5" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="124" t="s">
         <v>397</v>
       </c>
       <c r="C5" s="85"/>
@@ -13076,7 +13343,7 @@
       <c r="A6" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="85"/>
       <c r="D6" s="85"/>
       <c r="E6" s="96" t="s">
@@ -13097,7 +13364,7 @@
       <c r="A7" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="85"/>
       <c r="D7" s="85" t="s">
         <v>273</v>
@@ -13120,7 +13387,7 @@
       <c r="A8" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="85"/>
       <c r="D8" s="85"/>
       <c r="E8" s="26" t="s">
@@ -13141,7 +13408,7 @@
       <c r="A9" s="85" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="122"/>
+      <c r="B9" s="124"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="26" t="s">
@@ -13162,7 +13429,7 @@
       <c r="A10" s="85" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="122"/>
+      <c r="B10" s="124"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="26" t="s">
@@ -13183,7 +13450,7 @@
       <c r="A11" s="85" t="s">
         <v>283</v>
       </c>
-      <c r="B11" s="122"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="26" t="s">
@@ -13204,7 +13471,7 @@
       <c r="A12" s="85" t="s">
         <v>284</v>
       </c>
-      <c r="B12" s="122"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="96" t="s">
@@ -13225,7 +13492,7 @@
       <c r="A13" s="85" t="s">
         <v>285</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="96" t="s">
@@ -13246,7 +13513,7 @@
       <c r="A14" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="B14" s="122"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="96" t="s">
@@ -13267,7 +13534,7 @@
       <c r="A15" s="85" t="s">
         <v>287</v>
       </c>
-      <c r="B15" s="122"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="96" t="s">
@@ -13288,7 +13555,7 @@
       <c r="A16" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="B16" s="122"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="96" t="s">
@@ -13309,7 +13576,7 @@
       <c r="A17" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="B17" s="122"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="96" t="s">
@@ -13330,7 +13597,7 @@
       <c r="A18" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="B18" s="122"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="96" t="s">
@@ -13351,7 +13618,7 @@
       <c r="A19" s="85" t="s">
         <v>291</v>
       </c>
-      <c r="B19" s="122"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="96" t="s">
@@ -13372,7 +13639,7 @@
       <c r="A20" s="85" t="s">
         <v>292</v>
       </c>
-      <c r="B20" s="122"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="96" t="s">
@@ -13543,71 +13810,71 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H22">
-    <cfRule type="cellIs" dxfId="195" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="15" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="16" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="17" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="18" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="20" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="188" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:H27">
-    <cfRule type="cellIs" dxfId="181" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13631,7 +13898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13692,7 +13961,7 @@
       <c r="A3" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="136" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="85"/>
@@ -13717,7 +13986,7 @@
       <c r="A4" s="112" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="135"/>
+      <c r="B4" s="137"/>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="65" t="s">
@@ -13966,323 +14235,323 @@
       <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="141"/>
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
+      <c r="A16" s="114"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
       <c r="E16" s="70"/>
       <c r="F16" s="71"/>
       <c r="G16" s="71"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
     </row>
     <row r="17" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="141"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
+      <c r="A17" s="114"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
       <c r="E17" s="70"/>
       <c r="F17" s="71"/>
       <c r="G17" s="71"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
+      <c r="H17" s="114"/>
+      <c r="I17" s="114"/>
     </row>
     <row r="18" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="141"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
+      <c r="A18" s="114"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
       <c r="E18" s="70"/>
       <c r="F18" s="71"/>
       <c r="G18" s="71"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
     </row>
     <row r="19" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="141"/>
-      <c r="B19" s="141"/>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
+      <c r="A19" s="114"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
       <c r="E19" s="70"/>
       <c r="F19" s="71"/>
       <c r="G19" s="71"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="114"/>
     </row>
     <row r="20" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="141"/>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
+      <c r="A20" s="114"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="114"/>
+      <c r="D20" s="114"/>
       <c r="E20" s="70"/>
       <c r="F20" s="71"/>
       <c r="G20" s="71"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="114"/>
     </row>
     <row r="21" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="141"/>
-      <c r="B21" s="141"/>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
+      <c r="A21" s="114"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
       <c r="E21" s="70"/>
       <c r="F21" s="71"/>
       <c r="G21" s="71"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
+      <c r="H21" s="114"/>
+      <c r="I21" s="114"/>
     </row>
     <row r="22" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="141"/>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
+      <c r="A22" s="114"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="114"/>
       <c r="E22" s="70"/>
       <c r="F22" s="71"/>
       <c r="G22" s="71"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="114"/>
     </row>
     <row r="23" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="141"/>
-      <c r="B23" s="141"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
+      <c r="A23" s="114"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="114"/>
       <c r="E23" s="70"/>
       <c r="F23" s="71"/>
       <c r="G23" s="71"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="114"/>
     </row>
     <row r="24" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="141"/>
-      <c r="B24" s="141"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="141"/>
-      <c r="F24" s="141"/>
-      <c r="G24" s="141"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
+      <c r="A24" s="114"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="114"/>
+      <c r="I24" s="114"/>
     </row>
     <row r="25" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="141"/>
-      <c r="B25" s="141"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
+      <c r="A25" s="114"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="114"/>
       <c r="E25" s="70"/>
       <c r="F25" s="71"/>
       <c r="G25" s="71"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
+      <c r="H25" s="114"/>
+      <c r="I25" s="114"/>
     </row>
     <row r="26" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="141"/>
-      <c r="B26" s="141"/>
-      <c r="C26" s="141"/>
-      <c r="D26" s="141"/>
+      <c r="A26" s="114"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="114"/>
+      <c r="D26" s="114"/>
       <c r="E26" s="70"/>
       <c r="F26" s="71"/>
       <c r="G26" s="71"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
+      <c r="H26" s="114"/>
+      <c r="I26" s="114"/>
     </row>
     <row r="27" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="141"/>
-      <c r="B27" s="141"/>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
+      <c r="A27" s="114"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="114"/>
       <c r="E27" s="70"/>
       <c r="F27" s="71"/>
       <c r="G27" s="71"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="141"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="114"/>
     </row>
     <row r="28" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="141"/>
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
+      <c r="A28" s="114"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="114"/>
       <c r="E28" s="70"/>
       <c r="F28" s="71"/>
       <c r="G28" s="71"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="114"/>
     </row>
     <row r="29" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="141"/>
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="141"/>
+      <c r="A29" s="114"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
       <c r="E29" s="70"/>
       <c r="F29" s="71"/>
       <c r="G29" s="71"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
     </row>
     <row r="30" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="141"/>
-      <c r="B30" s="141"/>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
+      <c r="A30" s="114"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="114"/>
       <c r="E30" s="70"/>
       <c r="F30" s="71"/>
       <c r="G30" s="71"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="114"/>
     </row>
     <row r="31" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="141"/>
-      <c r="B31" s="141"/>
-      <c r="C31" s="141"/>
-      <c r="D31" s="141"/>
+      <c r="A31" s="114"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="114"/>
       <c r="E31" s="70"/>
       <c r="F31" s="71"/>
       <c r="G31" s="71"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="141"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="114"/>
     </row>
     <row r="32" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="141"/>
-      <c r="B32" s="141"/>
-      <c r="C32" s="141"/>
-      <c r="D32" s="141"/>
+      <c r="A32" s="114"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
       <c r="E32" s="70"/>
       <c r="F32" s="71"/>
       <c r="G32" s="71"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="141"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
     </row>
     <row r="33" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="141"/>
-      <c r="B33" s="141"/>
-      <c r="C33" s="141"/>
-      <c r="D33" s="141"/>
+      <c r="A33" s="114"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
       <c r="E33" s="70"/>
       <c r="F33" s="71"/>
       <c r="G33" s="71"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="114"/>
     </row>
     <row r="34" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="141"/>
-      <c r="B34" s="141"/>
-      <c r="C34" s="141"/>
-      <c r="D34" s="141"/>
+      <c r="A34" s="114"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="114"/>
       <c r="E34" s="70"/>
       <c r="F34" s="71"/>
       <c r="G34" s="71"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="141"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
     </row>
     <row r="35" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="141"/>
-      <c r="B35" s="141"/>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
+      <c r="A35" s="114"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="114"/>
       <c r="E35" s="70"/>
       <c r="F35" s="71"/>
       <c r="G35" s="71"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
+      <c r="H35" s="114"/>
+      <c r="I35" s="114"/>
     </row>
     <row r="36" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="141"/>
-      <c r="B36" s="141"/>
-      <c r="C36" s="141"/>
-      <c r="D36" s="141"/>
+      <c r="A36" s="114"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="70"/>
       <c r="F36" s="71"/>
       <c r="G36" s="71"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="114"/>
     </row>
     <row r="37" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="141"/>
-      <c r="B37" s="141"/>
-      <c r="C37" s="141"/>
-      <c r="D37" s="141"/>
+      <c r="A37" s="114"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="70"/>
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="141"/>
+      <c r="H37" s="114"/>
+      <c r="I37" s="114"/>
     </row>
     <row r="38" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="141"/>
-      <c r="B38" s="141"/>
-      <c r="C38" s="141"/>
-      <c r="D38" s="141"/>
+      <c r="A38" s="114"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="70"/>
       <c r="F38" s="71"/>
       <c r="G38" s="71"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="141"/>
+      <c r="H38" s="114"/>
+      <c r="I38" s="114"/>
     </row>
     <row r="39" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="141"/>
-      <c r="B39" s="141"/>
-      <c r="C39" s="141"/>
-      <c r="D39" s="141"/>
+      <c r="A39" s="114"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
       <c r="E39" s="70"/>
       <c r="F39" s="71"/>
       <c r="G39" s="71"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
+      <c r="H39" s="114"/>
+      <c r="I39" s="114"/>
     </row>
     <row r="40" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="141"/>
-      <c r="B40" s="141"/>
-      <c r="C40" s="141"/>
-      <c r="D40" s="141"/>
+      <c r="A40" s="114"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="114"/>
       <c r="E40" s="70"/>
       <c r="F40" s="71"/>
       <c r="G40" s="71"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141"/>
+      <c r="H40" s="114"/>
+      <c r="I40" s="114"/>
     </row>
     <row r="41" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="141"/>
-      <c r="B41" s="141"/>
-      <c r="C41" s="141"/>
-      <c r="D41" s="141"/>
+      <c r="A41" s="114"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="114"/>
       <c r="E41" s="70"/>
       <c r="F41" s="71"/>
       <c r="G41" s="71"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141"/>
+      <c r="H41" s="114"/>
+      <c r="I41" s="114"/>
     </row>
     <row r="42" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="141"/>
-      <c r="B42" s="141"/>
-      <c r="C42" s="141"/>
-      <c r="D42" s="141"/>
+      <c r="A42" s="114"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="114"/>
+      <c r="D42" s="114"/>
       <c r="E42" s="70"/>
       <c r="F42" s="71"/>
       <c r="G42" s="71"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
+      <c r="H42" s="114"/>
+      <c r="I42" s="114"/>
     </row>
     <row r="43" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="141"/>
-      <c r="B43" s="141"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="141"/>
+      <c r="A43" s="114"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="114"/>
       <c r="E43" s="70"/>
       <c r="F43" s="71"/>
       <c r="G43" s="71"/>
-      <c r="H43" s="141"/>
-      <c r="I43" s="141"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114"/>
     </row>
     <row r="44" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="141"/>
-      <c r="B44" s="141"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="141"/>
+      <c r="A44" s="114"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
       <c r="E44" s="70"/>
       <c r="F44" s="71"/>
       <c r="G44" s="71"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="141"/>
+      <c r="H44" s="114"/>
+      <c r="I44" s="114"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
@@ -14400,48 +14669,48 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="H3:H12">
-    <cfRule type="cellIs" dxfId="174" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="9" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="10" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="13" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H15">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="3" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="6" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14463,11 +14732,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8632243-8F65-4A22-8934-EB264B136ECB}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14480,58 +14747,728 @@
     <col min="7" max="7" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="91"/>
+    </row>
+    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="92" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A3" s="113" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="136" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>512</v>
+      </c>
+      <c r="H3" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="113" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="137"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="65" t="s">
+        <v>399</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="H4" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="113" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="65" t="s">
+        <v>398</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="H5" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="113" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="65" t="s">
+        <v>462</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>459</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>460</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="113" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="65" t="s">
+        <v>461</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="H7" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="113" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="65" t="s">
+        <v>465</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="H8" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A9" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="65" t="s">
+        <v>600</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>598</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>603</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A10" s="113" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="65" t="s">
+        <v>599</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>601</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>602</v>
+      </c>
+      <c r="H10" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A11" s="113" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="139" t="s">
-        <v>462</v>
-      </c>
-      <c r="F1" s="140" t="s">
-        <v>459</v>
-      </c>
-      <c r="G1" s="140" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="137" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="65" t="s">
+        <v>606</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>604</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="H11" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="113" t="s">
         <v>284</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="139" t="s">
-        <v>461</v>
-      </c>
-      <c r="F2" s="140" t="s">
-        <v>463</v>
-      </c>
-      <c r="G2" s="140" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="65" t="s">
+        <v>607</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>608</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>609</v>
+      </c>
+      <c r="H12" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="113" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="139" t="s">
-        <v>465</v>
-      </c>
-      <c r="F3" s="140" t="s">
-        <v>466</v>
-      </c>
-      <c r="G3" s="140" t="s">
-        <v>467</v>
-      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="65" t="s">
+        <v>610</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>613</v>
+      </c>
+      <c r="H13" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="65" t="s">
+        <v>614</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>615</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>616</v>
+      </c>
+      <c r="H14" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="113" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="65" t="s">
+        <v>618</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>617</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>619</v>
+      </c>
+      <c r="H15" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="113" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="65" t="s">
+        <v>620</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>622</v>
+      </c>
+      <c r="H16" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A17" s="113" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="65" t="s">
+        <v>623</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>624</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>625</v>
+      </c>
+      <c r="H17" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A18" s="113" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="65" t="s">
+        <v>626</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>627</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>628</v>
+      </c>
+      <c r="H18" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A19" s="113" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="65" t="s">
+        <v>629</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>630</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="H19" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A20" s="113" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="65" t="s">
+        <v>632</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>631</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>641</v>
+      </c>
+      <c r="H20" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A21" s="113" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="65" t="s">
+        <v>633</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>604</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="H21" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="113" t="s">
+        <v>453</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="65" t="s">
+        <v>634</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>635</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>609</v>
+      </c>
+      <c r="H22" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="113" t="s">
+        <v>454</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>639</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>613</v>
+      </c>
+      <c r="H23" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="113" t="s">
+        <v>455</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="65" t="s">
+        <v>614</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>615</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>616</v>
+      </c>
+      <c r="H24" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="113" t="s">
+        <v>456</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="65" t="s">
+        <v>637</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>638</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>642</v>
+      </c>
+      <c r="H25" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="113" t="s">
+        <v>457</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="65" t="s">
+        <v>620</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>622</v>
+      </c>
+      <c r="H26" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A27" s="113" t="s">
+        <v>458</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="65" t="s">
+        <v>623</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>643</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>625</v>
+      </c>
+      <c r="H27" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A28" s="113" t="s">
+        <v>558</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="65" t="s">
+        <v>626</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>627</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>628</v>
+      </c>
+      <c r="H28" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="113" t="s">
+        <v>559</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="65" t="s">
+        <v>644</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>649</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="H29" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="113" t="s">
+        <v>560</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="65" t="s">
+        <v>646</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>647</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>648</v>
+      </c>
+      <c r="H30" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="113" t="s">
+        <v>561</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="65" t="s">
+        <v>650</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>651</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>652</v>
+      </c>
+      <c r="H31" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="113" t="s">
+        <v>562</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
+  <conditionalFormatting sqref="H3:H32">
+    <cfRule type="cellIs" dxfId="160" priority="8" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="10" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="11" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="12" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="13" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="14" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71F8564F-CA59-43E6-AE33-23877ACE3433}">
+          <x14:formula1>
+            <xm:f>Info!$A$3:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>H3:H32</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ingest test cases added
</commit_message>
<xml_diff>
--- a/App_QC_Regression_Test_Case.xlsx
+++ b/App_QC_Regression_Test_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shail\Documents\BlueStackTestFiles\automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94DA917-BDC4-4CC7-A0B1-A96C257F09FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AA10B0-D5B0-434B-B1F8-B3C70E277EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="892" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="892" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Page" sheetId="14" r:id="rId1"/>
@@ -13957,8 +13957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:I5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14774,6 +14774,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -14793,8 +14794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8632243-8F65-4A22-8934-EB264B136ECB}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>